<commit_message>
resize font and change format
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC IT-Server\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55DAE6C-9950-430B-9605-78DD4934C7C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09683224-53CD-44ED-AE0A-BC9E9B0F89F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Kode Mesin</t>
   </si>
@@ -266,13 +266,16 @@
   </si>
   <si>
     <t>FIELD7</t>
+  </si>
+  <si>
+    <t>tes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -294,6 +297,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +380,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +602,7 @@
   <dimension ref="A1:K237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -613,7 +624,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -663,7 +674,12 @@
       <c r="H2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K2" s="5" t="s">
         <v>25</v>
       </c>
@@ -693,7 +709,12 @@
       <c r="H3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
@@ -723,7 +744,12 @@
       <c r="H4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K4" s="5" t="s">
         <v>25</v>
       </c>
@@ -753,7 +779,12 @@
       <c r="H5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K5" s="5" t="s">
         <v>25</v>
       </c>
@@ -783,7 +814,12 @@
       <c r="H6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K6" s="5" t="s">
         <v>25</v>
       </c>
@@ -813,7 +849,12 @@
       <c r="H7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K7" s="5" t="s">
         <v>25</v>
       </c>
@@ -843,7 +884,12 @@
       <c r="H8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K8" s="5" t="s">
         <v>25</v>
       </c>
@@ -873,7 +919,12 @@
       <c r="H9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K9" s="5" t="s">
         <v>25</v>
       </c>
@@ -903,7 +954,12 @@
       <c r="H10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K10" s="5" t="s">
         <v>25</v>
       </c>
@@ -933,7 +989,12 @@
       <c r="H11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="K11" s="5" t="s">
         <v>25</v>
       </c>
@@ -3541,6 +3602,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>